<commit_message>
Minor edits to Computer Sys Functions Spreadsheet
</commit_message>
<xml_diff>
--- a/Documents/UUV Computer Systems Functions.xlsx
+++ b/Documents/UUV Computer Systems Functions.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve">System</t>
   </si>
@@ -49,10 +49,13 @@
     <t xml:space="preserve">Raspberry Pi</t>
   </si>
   <si>
-    <t xml:space="preserve">Receive commands from surface</t>
+    <t xml:space="preserve">Receive commands from surface, send commands to Arduino</t>
   </si>
   <si>
     <t xml:space="preserve">Arduino</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reading sensor data</t>
   </si>
   <si>
     <t xml:space="preserve">ESC</t>
@@ -73,6 +76,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -94,6 +98,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -264,7 +269,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="26.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -322,14 +327,16 @@
       <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="4"/>
+      <c r="B7" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated computer systems spreadsheet
</commit_message>
<xml_diff>
--- a/Documents/UUV Computer Systems Functions.xlsx
+++ b/Documents/UUV Computer Systems Functions.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
   <si>
     <t xml:space="preserve">System</t>
   </si>
@@ -28,18 +28,27 @@
     <t xml:space="preserve">Tasks</t>
   </si>
   <si>
+    <t xml:space="preserve">Language</t>
+  </si>
+  <si>
     <t xml:space="preserve">Gamepad/Controller</t>
   </si>
   <si>
     <t xml:space="preserve">Send control input to surface computer</t>
   </si>
   <si>
+    <t xml:space="preserve">N/A</t>
+  </si>
+  <si>
     <t xml:space="preserve">Surface Operator Computer</t>
   </si>
   <si>
     <t xml:space="preserve">Relay control input to onboard computer (RasPi)</t>
   </si>
   <si>
+    <t xml:space="preserve">Python</t>
+  </si>
+  <si>
     <t xml:space="preserve">Send commands to onboard computer</t>
   </si>
   <si>
@@ -49,19 +58,55 @@
     <t xml:space="preserve">Raspberry Pi</t>
   </si>
   <si>
-    <t xml:space="preserve">Receive commands from surface, send commands to Arduino</t>
+    <t xml:space="preserve">Receive commands from surface, send commands to Arduino  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Receive controller input from surface, interpret controller input, send commands to Arduino</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Receive sensor data from Arduino, send sensor data to surface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Process sensor data, use sensor data to control vehicle (adjust camera angle, stabilize attitude, etc.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Receive camera feed from camera, stream camera feed to surface</t>
   </si>
   <si>
     <t xml:space="preserve">Arduino</t>
   </si>
   <si>
-    <t xml:space="preserve">Reading sensor data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ESC</t>
+    <t xml:space="preserve">Read sensor data, send sensor data to onboard computer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C++</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Receive commands from onboard computer, send control signals to ESCs, servos, etc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESC (Electronic Speed Controller)</t>
   </si>
   <si>
     <t xml:space="preserve">Relay motor control signals from Arduino to motor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6-axis sensor (Gyroscope &amp; Accelerometer)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Send acceleration &amp; rotation data to Arduino</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thermistor (Temperature sensor)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Send temperature data to Arduino</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Camera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Send video feed to onboard computer</t>
   </si>
 </sst>
 </file>
@@ -71,7 +116,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -99,6 +144,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -168,7 +218,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -178,15 +228,19 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -266,17 +320,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="26.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.15"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="3" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.76"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -286,62 +341,155 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
-        <v>6</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" customFormat="false" ht="31.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="4" t="s">
+    </row>
+    <row r="7" customFormat="false" ht="34.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4"/>
+      <c r="B7" s="5" t="s">
         <v>13</v>
       </c>
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" customFormat="false" ht="33.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4"/>
+      <c r="B8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="4"/>
+    </row>
+    <row r="9" customFormat="false" ht="31.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4"/>
+      <c r="B9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="4"/>
+    </row>
+    <row r="10" customFormat="false" ht="31.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4"/>
+      <c r="B10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="4"/>
+    </row>
+    <row r="11" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="31.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4"/>
+      <c r="B12" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="4"/>
+    </row>
+    <row r="13" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="32.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="34.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="30.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="6">
     <mergeCell ref="A3:A5"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="C6:C10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="C11:C12"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>